<commit_message>
What was Shown to Dave Egbers
Submission includes the Differences in 3 point selection between VAV and FPB.
</commit_message>
<xml_diff>
--- a/products.xlsx
+++ b/products.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\UserData\lanzaa\Documents\GitHub\Flask_Sites\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D7214BF8-B902-43E3-9902-5CD9E585E130}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AB8B9E5B-356A-4590-A566-8465226B1116}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{8E159910-7E01-42DB-B7FB-B682CA6AF500}"/>
   </bookViews>
@@ -33,13 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="14">
-  <si>
-    <t>3pt Floating Actuator Key</t>
-  </si>
-  <si>
-    <t>3pt Floating Actuator Value</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="315" uniqueCount="63">
   <si>
     <t>X</t>
   </si>
@@ -59,22 +53,175 @@
     <t>None</t>
   </si>
   <si>
-    <t>6-10" Duct</t>
-  </si>
-  <si>
-    <t>12-14" Duct</t>
-  </si>
-  <si>
-    <t>Slow: GDE131.1P</t>
-  </si>
-  <si>
-    <t>Fast: GDE191.1P</t>
-  </si>
-  <si>
-    <t>Slow: GDE121.1P</t>
-  </si>
-  <si>
-    <t>Fast: GDE181.1P</t>
+    <t>Functionality Key</t>
+  </si>
+  <si>
+    <t>Functionality Value</t>
+  </si>
+  <si>
+    <t>VAV</t>
+  </si>
+  <si>
+    <t>FCU</t>
+  </si>
+  <si>
+    <t>FPB</t>
+  </si>
+  <si>
+    <t>WSHP</t>
+  </si>
+  <si>
+    <t>Lab Tracking</t>
+  </si>
+  <si>
+    <t>Fumehood</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> </t>
+  </si>
+  <si>
+    <t>Central Function</t>
+  </si>
+  <si>
+    <t>Supply Damper</t>
+  </si>
+  <si>
+    <t>Exhuast Damper</t>
+  </si>
+  <si>
+    <t>Chilled Water Valve</t>
+  </si>
+  <si>
+    <t>Chilled Beam Valve</t>
+  </si>
+  <si>
+    <t>Y1Y2 VAV Key</t>
+  </si>
+  <si>
+    <t>Y1Y2 VAV Value</t>
+  </si>
+  <si>
+    <t>Y3Y4 VAV Key</t>
+  </si>
+  <si>
+    <t>Y3Y4 VAV Value</t>
+  </si>
+  <si>
+    <t>Y5Y6 VAV Key</t>
+  </si>
+  <si>
+    <t>Y5Y6 VAV Value</t>
+  </si>
+  <si>
+    <t>Y7Y8 VAV Key</t>
+  </si>
+  <si>
+    <t>Dual Duct 1/2</t>
+  </si>
+  <si>
+    <t>E</t>
+  </si>
+  <si>
+    <t>Chilled Beam Active</t>
+  </si>
+  <si>
+    <t>Cooling Coil Valve</t>
+  </si>
+  <si>
+    <t>Heating/Cooling Coil</t>
+  </si>
+  <si>
+    <t>F</t>
+  </si>
+  <si>
+    <t>Heating Coil</t>
+  </si>
+  <si>
+    <t>Electric 2 Stage</t>
+  </si>
+  <si>
+    <t>Radiant Ceiling Chilled</t>
+  </si>
+  <si>
+    <t>Radiant Heating/Chilled</t>
+  </si>
+  <si>
+    <t>Heat/Chilled Beam Passive</t>
+  </si>
+  <si>
+    <t>Radiator Fin Tube</t>
+  </si>
+  <si>
+    <t>S</t>
+  </si>
+  <si>
+    <t>G</t>
+  </si>
+  <si>
+    <t>H</t>
+  </si>
+  <si>
+    <t>I</t>
+  </si>
+  <si>
+    <t>J</t>
+  </si>
+  <si>
+    <t>K</t>
+  </si>
+  <si>
+    <t>L</t>
+  </si>
+  <si>
+    <t>Windows</t>
+  </si>
+  <si>
+    <t>General 3Pt Floating</t>
+  </si>
+  <si>
+    <t>Y7Y8 VAV Value</t>
+  </si>
+  <si>
+    <t>Y1Y2 FPB Key</t>
+  </si>
+  <si>
+    <t>Y1Y2 FPB Value</t>
+  </si>
+  <si>
+    <t>Y3Y4 FPB Key</t>
+  </si>
+  <si>
+    <t>Y3Y4 FPB Value</t>
+  </si>
+  <si>
+    <t>Y5Y6 FPB Key</t>
+  </si>
+  <si>
+    <t>Y5Y6 FPB Value</t>
+  </si>
+  <si>
+    <t>Y7Y8 FPB Key</t>
+  </si>
+  <si>
+    <t>Y7Y8 FPB Value</t>
+  </si>
+  <si>
+    <t>Fan Speed 2 Stage</t>
+  </si>
+  <si>
+    <t>M</t>
+  </si>
+  <si>
+    <t>Radiant Heating</t>
+  </si>
+  <si>
+    <t>N</t>
+  </si>
+  <si>
+    <t>Chilled Beam Passive</t>
+  </si>
+  <si>
+    <t>O</t>
   </si>
 </sst>
 </file>
@@ -429,80 +576,1034 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9912844E-43B3-478C-9942-25BB405BFB37}">
-  <dimension ref="A1:B8"/>
+  <dimension ref="A1:R19"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A8" sqref="A8"/>
+      <selection activeCell="J7" sqref="J7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="30" style="1" customWidth="1"/>
-    <col min="2" max="2" width="29.7109375" style="1" customWidth="1"/>
+    <col min="1" max="1" width="16.42578125" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="18.42578125" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="24.7109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="26.7109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="5" max="6" width="26.7109375" style="1" customWidth="1"/>
+    <col min="7" max="7" width="27.7109375" style="1" customWidth="1"/>
+    <col min="8" max="8" width="26.7109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="9" max="10" width="26.7109375" style="1" customWidth="1"/>
+    <col min="11" max="11" width="24.7109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="26.7109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="13" max="14" width="26.7109375" style="1" customWidth="1"/>
+    <col min="15" max="15" width="24.7109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="26.7109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="23.42578125" style="1" customWidth="1"/>
+    <col min="18" max="18" width="23.5703125" style="1" customWidth="1"/>
+    <col min="19" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="J1" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="K1" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="L1" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="M1" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="N1" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="O1" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="P1" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="Q1" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="R1" s="1" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="2" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A2" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="B2" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A2" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="B2" s="1" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C2" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="E2" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="F2" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="G2" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="H2" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="I2" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="J2" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="K2" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="L2" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="M2" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="N2" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="O2" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="P2" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="Q2" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="R2" s="1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="B3" s="1" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B3" s="1">
+        <v>1</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="D3" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="E3" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="F3" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="G3" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="H3" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="I3" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="J3" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="K3" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="L3" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="M3" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="N3" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="O3" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="P3" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="Q3" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="R3" s="1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="B4" s="1" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B4" s="1">
+        <v>2</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="D4" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="E4" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="F4" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="G4" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="H4" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="I4" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="J4" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="K4" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="L4" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="M4" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="N4" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="O4" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="P4" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="Q4" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="R4" s="1" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="5" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="B5" s="1" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B5" s="1">
+        <v>3</v>
+      </c>
+      <c r="C5" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="D5" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E5" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="F5" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="G5" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="H5" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="I5" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="J5" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="K5" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="L5" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="M5" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="N5" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="O5" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="P5" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="Q5" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="R5" s="1" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="6" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="B6" s="1" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B6" s="1">
+        <v>4</v>
+      </c>
+      <c r="C6" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="D6" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="E6" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="F6" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="G6" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="H6" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="I6" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="J6" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="K6" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="L6" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="M6" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="N6" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="O6" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="P6" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="Q6" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="R6" s="1" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="7" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="B7" s="1" t="s">
+      <c r="B7" s="1">
         <v>5</v>
       </c>
-    </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C7" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="D7" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="E7" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="F7" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="G7" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="H7" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="I7" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="J7" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="K7" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="L7" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="M7" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="N7" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="O7" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="P7" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="Q7" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="R7" s="1" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="8" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="B8" s="1" t="s">
+      <c r="B8" s="1">
         <v>6</v>
+      </c>
+      <c r="C8" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="D8" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="E8" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="F8" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="G8" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="H8" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="I8" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="J8" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="K8" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="L8" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="M8" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="N8" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="O8" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="P8" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="Q8" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="R8" s="1" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="9" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A9" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="B9" s="1">
+        <v>7</v>
+      </c>
+      <c r="C9" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="D9" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="E9" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="F9" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="G9" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="H9" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="I9" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="J9" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="K9" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="L9" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="M9" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="N9" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="O9" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="P9" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="Q9" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="R9" s="1" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="10" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="C10" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="D10" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="E10" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="F10" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="G10" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="H10" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="I10" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="J10" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="K10" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="L10" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="M10" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="N10" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="O10" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="P10" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="Q10" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="R10" s="1" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="11" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="C11" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="D11" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="E11" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="F11" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="G11" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="H11" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="I11" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="J11" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="K11" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="L11" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="M11" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="N11" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="O11" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="P11" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="Q11" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="R11" s="1" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="12" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="C12" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="D12" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="E12" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="F12" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="G12" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="H12" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="I12" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="J12" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="K12" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="L12" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="M12" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="N12" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="O12" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="P12" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="Q12" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="R12" s="1" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="13" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="C13" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="D13" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="E13" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="F13" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="G13" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="H13" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="I13" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="J13" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="K13" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="L13" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="M13" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="N13" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="O13" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="P13" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="Q13" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="R13" s="1" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="14" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="C14" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="D14" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="E14" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="F14" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="G14" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="H14" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="I14" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="J14" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="K14" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="L14" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="M14" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="N14" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="O14" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="P14" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="Q14" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="R14" s="1" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="15" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="C15" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="D15" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="E15" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="F15" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="G15" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="H15" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="I15" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="J15" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="K15" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="L15" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="M15" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="N15" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="O15" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="P15" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="Q15" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="R15" s="1" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="16" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="C16" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="D16" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="E16" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="F16" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="G16" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="H16" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="I16" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="J16" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="K16" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="L16" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="M16" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="N16" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="O16" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="P16" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="Q16" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="R16" s="1" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="17" spans="3:18" x14ac:dyDescent="0.25">
+      <c r="C17" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="D17" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="E17" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="F17" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="G17" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="H17" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="I17" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="J17" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="K17" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="L17" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="M17" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="N17" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="O17" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="P17" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="Q17" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="R17" s="1" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="18" spans="3:18" x14ac:dyDescent="0.25">
+      <c r="C18" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="D18" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="E18" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="F18" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="G18" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="H18" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="I18" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="J18" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="K18" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="L18" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="M18" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="N18" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="O18" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="P18" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="Q18" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="R18" s="1" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="19" spans="3:18" x14ac:dyDescent="0.25">
+      <c r="C19" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="D19" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="E19" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="F19" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="G19" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="H19" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="I19" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="J19" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="K19" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="L19" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="M19" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="N19" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="O19" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="P19" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="Q19" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="R19" s="1" t="s">
+        <v>62</v>
       </c>
     </row>
   </sheetData>

</xml_diff>